<commit_message>
Add nap tien vao tai khoan
</commit_message>
<xml_diff>
--- a/doc/MaidProject-API.xlsx
+++ b/doc/MaidProject-API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="1"/>
+    <workbookView xWindow="15740" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1383,13 +1383,13 @@
     </row>
     <row r="29" spans="3:6" ht="180" x14ac:dyDescent="0.2">
       <c r="C29" s="28"/>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="17" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>